<commit_message>
updated complete fiscal year of 81.82
</commit_message>
<xml_diff>
--- a/public/data/customoffice_trade_allyr.xlsx
+++ b/public/data/customoffice_trade_allyr.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AO30"/>
+  <dimension ref="A1:AO29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,7 +532,7 @@
         <v>BHADRAPUR</v>
       </c>
       <c r="B2" t="str">
-        <v>499235</v>
+        <v>524123</v>
       </c>
       <c r="C2" t="str">
         <v>0.03</v>
@@ -657,16 +657,16 @@
         <v>BHAIRAHAWA</v>
       </c>
       <c r="B3" t="str">
-        <v>240485392</v>
+        <v>263815067</v>
       </c>
       <c r="C3" t="str">
         <v>14.62</v>
       </c>
       <c r="D3" t="str">
-        <v>18589373</v>
+        <v>20922356</v>
       </c>
       <c r="E3" t="str">
-        <v>7.51</v>
+        <v>7.55</v>
       </c>
       <c r="F3" t="str">
         <v>242636057</v>
@@ -782,16 +782,16 @@
         <v>BIRATNAGAR</v>
       </c>
       <c r="B4" t="str">
-        <v>189861005</v>
+        <v>210419433</v>
       </c>
       <c r="C4" t="str">
-        <v>11.54</v>
+        <v>11.66</v>
       </c>
       <c r="D4" t="str">
-        <v>65187815</v>
+        <v>74017141</v>
       </c>
       <c r="E4" t="str">
-        <v>26.33</v>
+        <v>26.72</v>
       </c>
       <c r="F4" t="str">
         <v>168298937</v>
@@ -907,16 +907,16 @@
         <v>BIRGUNJ</v>
       </c>
       <c r="B5" t="str">
-        <v>564757719</v>
+        <v>625087176</v>
       </c>
       <c r="C5" t="str">
-        <v>34.34</v>
+        <v>34.65</v>
       </c>
       <c r="D5" t="str">
-        <v>91507114</v>
+        <v>101838151</v>
       </c>
       <c r="E5" t="str">
-        <v>36.96</v>
+        <v>36.76</v>
       </c>
       <c r="F5" t="str">
         <v>546438040</v>
@@ -1032,7 +1032,7 @@
         <v>CHOBHAR</v>
       </c>
       <c r="B6" t="str">
-        <v>1521071</v>
+        <v>1695556</v>
       </c>
       <c r="C6" t="str">
         <v>0.09</v>
@@ -1157,16 +1157,16 @@
         <v>DRYPORT</v>
       </c>
       <c r="B7" t="str">
-        <v>204921034</v>
+        <v>223117105</v>
       </c>
       <c r="C7" t="str">
-        <v>12.46</v>
+        <v>12.37</v>
       </c>
       <c r="D7" t="str">
-        <v>4841263</v>
+        <v>5496403</v>
       </c>
       <c r="E7" t="str">
-        <v>1.96</v>
+        <v>1.98</v>
       </c>
       <c r="F7" t="str">
         <v>203636739</v>
@@ -1282,13 +1282,13 @@
         <v>GAUR</v>
       </c>
       <c r="B8" t="str">
-        <v>1017882</v>
+        <v>1163670</v>
       </c>
       <c r="C8" t="str">
         <v>0.06</v>
       </c>
       <c r="D8" t="str">
-        <v>13858</v>
+        <v>16751</v>
       </c>
       <c r="E8" t="str">
         <v>0.01</v>
@@ -1532,16 +1532,16 @@
         <v>JALESHWOR</v>
       </c>
       <c r="B10" t="str">
-        <v>9078307</v>
+        <v>9547920</v>
       </c>
       <c r="C10" t="str">
-        <v>0.55</v>
+        <v>0.53</v>
       </c>
       <c r="D10" t="str">
-        <v>2886612</v>
+        <v>3713720</v>
       </c>
       <c r="E10" t="str">
-        <v>1.17</v>
+        <v>1.34</v>
       </c>
       <c r="F10" t="str">
         <v>10613005</v>
@@ -1657,7 +1657,7 @@
         <v>JANAKPUR</v>
       </c>
       <c r="B11" t="str">
-        <v>1517239</v>
+        <v>1649387</v>
       </c>
       <c r="C11" t="str">
         <v>0.09</v>
@@ -1782,16 +1782,16 @@
         <v>KAILALI</v>
       </c>
       <c r="B12" t="str">
-        <v>22341243</v>
+        <v>24625736</v>
       </c>
       <c r="C12" t="str">
         <v>1.36</v>
       </c>
       <c r="D12" t="str">
-        <v>982910</v>
+        <v>1151744</v>
       </c>
       <c r="E12" t="str">
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
       <c r="F12" t="str">
         <v>22893132</v>
@@ -1907,13 +1907,13 @@
         <v>KANCHANPUR</v>
       </c>
       <c r="B13" t="str">
-        <v>1692805</v>
+        <v>1819722</v>
       </c>
       <c r="C13" t="str">
         <v>0.1</v>
       </c>
       <c r="D13" t="str">
-        <v>6048</v>
+        <v>6915</v>
       </c>
       <c r="E13" t="str">
         <v>0</v>
@@ -2032,16 +2032,16 @@
         <v>KRISHNANAGAR</v>
       </c>
       <c r="B14" t="str">
-        <v>22624316</v>
+        <v>24298575</v>
       </c>
       <c r="C14" t="str">
-        <v>1.38</v>
+        <v>1.35</v>
       </c>
       <c r="D14" t="str">
-        <v>2239452</v>
+        <v>2395931</v>
       </c>
       <c r="E14" t="str">
-        <v>0.9</v>
+        <v>0.86</v>
       </c>
       <c r="F14" t="str">
         <v>21905642</v>
@@ -2157,7 +2157,7 @@
         <v>MAHESHPAUR</v>
       </c>
       <c r="B15" t="str">
-        <v>526718</v>
+        <v>580890</v>
       </c>
       <c r="C15" t="str">
         <v>0.03</v>
@@ -2282,16 +2282,16 @@
         <v>MECHI</v>
       </c>
       <c r="B16" t="str">
-        <v>43354085</v>
+        <v>47259336</v>
       </c>
       <c r="C16" t="str">
-        <v>2.64</v>
+        <v>2.62</v>
       </c>
       <c r="D16" t="str">
-        <v>23282092</v>
+        <v>25138286</v>
       </c>
       <c r="E16" t="str">
-        <v>9.4</v>
+        <v>9.07</v>
       </c>
       <c r="F16" t="str">
         <v>44644832</v>
@@ -2407,16 +2407,16 @@
         <v>NEPALGUNJ</v>
       </c>
       <c r="B17" t="str">
-        <v>71230735</v>
+        <v>77577272</v>
       </c>
       <c r="C17" t="str">
-        <v>4.33</v>
+        <v>4.3</v>
       </c>
       <c r="D17" t="str">
-        <v>2851550</v>
+        <v>3208252</v>
       </c>
       <c r="E17" t="str">
-        <v>1.15</v>
+        <v>1.16</v>
       </c>
       <c r="F17" t="str">
         <v>70248790</v>
@@ -2532,13 +2532,13 @@
         <v>PASHUPATINAGAR</v>
       </c>
       <c r="B18" t="str">
-        <v>1021</v>
+        <v>1061</v>
       </c>
       <c r="C18" t="str">
         <v>0</v>
       </c>
       <c r="D18" t="str">
-        <v>47957</v>
+        <v>63071</v>
       </c>
       <c r="E18" t="str">
         <v>0.02</v>
@@ -2657,7 +2657,7 @@
         <v>RAJBIRAJ</v>
       </c>
       <c r="B19" t="str">
-        <v>196073</v>
+        <v>207862</v>
       </c>
       <c r="C19" t="str">
         <v>0.01</v>
@@ -2782,16 +2782,16 @@
         <v>RASUWA</v>
       </c>
       <c r="B20" t="str">
-        <v>80914823</v>
+        <v>85232360</v>
       </c>
       <c r="C20" t="str">
-        <v>4.92</v>
+        <v>4.72</v>
       </c>
       <c r="D20" t="str">
-        <v>1961403</v>
+        <v>2045261</v>
       </c>
       <c r="E20" t="str">
-        <v>0.79</v>
+        <v>0.74</v>
       </c>
       <c r="F20" t="str">
         <v>60910260</v>
@@ -2907,16 +2907,16 @@
         <v>SARLAHI</v>
       </c>
       <c r="B21" t="str">
-        <v>3228630</v>
+        <v>3356618</v>
       </c>
       <c r="C21" t="str">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="D21" t="str">
-        <v>878102</v>
+        <v>896460</v>
       </c>
       <c r="E21" t="str">
-        <v>0.35</v>
+        <v>0.32</v>
       </c>
       <c r="F21" t="str">
         <v>2573340</v>
@@ -3032,7 +3032,7 @@
         <v>SATI</v>
       </c>
       <c r="B22" t="str">
-        <v>458009</v>
+        <v>470248</v>
       </c>
       <c r="C22" t="str">
         <v>0.03</v>
@@ -3157,7 +3157,7 @@
         <v>SIRAHA</v>
       </c>
       <c r="B23" t="str">
-        <v>457707</v>
+        <v>494748</v>
       </c>
       <c r="C23" t="str">
         <v>0.03</v>
@@ -3282,7 +3282,7 @@
         <v>SUNSARI</v>
       </c>
       <c r="B24" t="str">
-        <v>1966638</v>
+        <v>2116382</v>
       </c>
       <c r="C24" t="str">
         <v>0.12</v>
@@ -3407,10 +3407,10 @@
         <v>SUTHAULI</v>
       </c>
       <c r="B25" t="str">
-        <v>4584396</v>
+        <v>5196057</v>
       </c>
       <c r="C25" t="str">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
       <c r="D25" t="str">
         <v>0</v>
@@ -3532,10 +3532,10 @@
         <v>TATOPANI</v>
       </c>
       <c r="B26" t="str">
-        <v>46893581</v>
+        <v>50395862</v>
       </c>
       <c r="C26" t="str">
-        <v>2.85</v>
+        <v>2.79</v>
       </c>
       <c r="D26" t="str">
         <v>0</v>
@@ -3657,7 +3657,7 @@
         <v>THADHI</v>
       </c>
       <c r="B27" t="str">
-        <v>24115</v>
+        <v>24385</v>
       </c>
       <c r="C27" t="str">
         <v>0</v>
@@ -3782,13 +3782,13 @@
         <v>TI_AIRPORT</v>
       </c>
       <c r="B28" t="str">
-        <v>130563305</v>
+        <v>143365575</v>
       </c>
       <c r="C28" t="str">
-        <v>7.94</v>
+        <v>7.95</v>
       </c>
       <c r="D28" t="str">
-        <v>32293769</v>
+        <v>36118864</v>
       </c>
       <c r="E28" t="str">
         <v>13.04</v>
@@ -3907,7 +3907,7 @@
         <v>TRIVENI</v>
       </c>
       <c r="B29" t="str">
-        <v>575</v>
+        <v>679</v>
       </c>
       <c r="C29" t="str">
         <v>0</v>
@@ -4024,50 +4024,12 @@
         <v/>
       </c>
       <c r="AO29" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="30">
-      <c r="Z30" t="str">
-        <v/>
-      </c>
-      <c r="AA30" t="str">
-        <v/>
-      </c>
-      <c r="AB30" t="str">
-        <v/>
-      </c>
-      <c r="AC30" t="str">
-        <v/>
-      </c>
-      <c r="AD30" t="str">
-        <v/>
-      </c>
-      <c r="AE30" t="str">
-        <v/>
-      </c>
-      <c r="AF30" t="str">
-        <v/>
-      </c>
-      <c r="AG30" t="str">
-        <v/>
-      </c>
-      <c r="AH30" t="str">
-        <v/>
-      </c>
-      <c r="AI30" t="str">
-        <v/>
-      </c>
-      <c r="AJ30" t="str">
-        <v/>
-      </c>
-      <c r="AK30" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AO30"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AO29"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>